<commit_message>
Insert some logo and favico
</commit_message>
<xml_diff>
--- a/DB/DB.xlsx
+++ b/DB/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table List" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="59">
   <si>
     <t>DB NAME</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>prefix</t>
+  </si>
+  <si>
+    <t>agree</t>
+  </si>
+  <si>
+    <t>refer</t>
   </si>
 </sst>
 </file>
@@ -310,11 +316,11 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -547,7 +553,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:J14" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:J15" totalsRowShown="0" headerRowDxfId="54">
   <tableColumns count="10">
     <tableColumn id="1" name="Stt" dataDxfId="53">
       <calculatedColumnFormula>ROW()-3</calculatedColumnFormula>
@@ -1155,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,11 +1183,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1222,7 +1228,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A12" si="0">ROW()-3</f>
+        <f t="shared" ref="A4:A13" si="0">ROW()-3</f>
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1248,12 +1254,12 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <f t="shared" si="0"/>
+      <c r="A5" s="11">
+        <f>ROW()-3</f>
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>25</v>
@@ -1274,7 +1280,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>25</v>
@@ -1295,13 +1301,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="2">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1316,13 +1322,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="2">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1337,23 +1343,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="5">
-        <v>1</v>
-      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1362,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>26</v>
@@ -1374,7 +1376,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="5">
         <v>1</v>
@@ -1387,19 +1389,23 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1408,7 +1414,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>27</v>
@@ -1424,10 +1430,19 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1446,6 +1461,18 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1484,11 +1511,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1777,7 +1804,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,11 +1823,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1841,7 +1868,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A11" si="0">ROW()-3</f>
+        <f t="shared" ref="A4:A13" si="0">ROW()-3</f>
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1916,23 +1943,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="5">
-        <v>2</v>
-      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1941,7 +1964,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>26</v>
@@ -1953,10 +1976,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="I8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="6"/>
     </row>
@@ -1966,7 +1989,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>26</v>
@@ -1977,12 +2000,8 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="5">
-        <v>1</v>
-      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1991,19 +2010,23 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1</v>
+      </c>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2012,26 +2035,39 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2040,10 +2076,19 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -2080,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2100,11 +2145,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2171,7 +2216,7 @@
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <f>ROW()-3</f>
         <v>2</v>
       </c>
@@ -2379,11 +2424,11 @@
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>

</xml_diff>

<commit_message>
change some name columns
</commit_message>
<xml_diff>
--- a/DB/DB.xlsx
+++ b/DB/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Table List" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="61">
   <si>
     <t>DB NAME</t>
   </si>
@@ -97,12 +97,6 @@
     <t>del_flg</t>
   </si>
   <si>
-    <t>create_date</t>
-  </si>
-  <si>
-    <t>update_date</t>
-  </si>
-  <si>
     <t>bigint</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>updat_date</t>
-  </si>
-  <si>
     <t>1: Main(Login), 2: child</t>
   </si>
   <si>
@@ -206,6 +197,21 @@
   </si>
   <si>
     <t>refer</t>
+  </si>
+  <si>
+    <t>from_refer</t>
+  </si>
+  <si>
+    <t>gavatar</t>
+  </si>
+  <si>
+    <t>create_at</t>
+  </si>
+  <si>
+    <t>update_at</t>
+  </si>
+  <si>
+    <t>updat_at</t>
   </si>
 </sst>
 </file>
@@ -553,7 +559,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:J15" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:J19" totalsRowShown="0" headerRowDxfId="54">
   <tableColumns count="10">
     <tableColumn id="1" name="Stt" dataDxfId="53">
       <calculatedColumnFormula>ROW()-3</calculatedColumnFormula>
@@ -917,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -940,7 +946,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
@@ -966,7 +972,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -975,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -984,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -993,7 +999,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -1161,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,44 +1234,44 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A13" si="0">ROW()-3</f>
+        <f t="shared" ref="A4:A17" si="0">ROW()-3</f>
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <f>ROW()-3</f>
+      <c r="A5" s="4">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1280,13 +1286,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1301,13 +1307,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1322,13 +1328,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1343,10 +1349,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2">
         <v>50</v>
@@ -1364,23 +1370,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="5">
-        <v>1</v>
-      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1389,23 +1391,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1</v>
-      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1414,13 +1412,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1435,13 +1433,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" s="2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1451,28 +1449,120 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
       <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1492,7 +1582,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +1602,7 @@
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -1560,22 +1650,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -1590,7 +1680,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2">
         <v>20</v>
@@ -1608,10 +1698,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2">
         <v>255</v>
@@ -1629,10 +1719,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2">
         <v>255</v>
@@ -1650,10 +1740,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
         <v>15</v>
@@ -1671,10 +1761,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2">
         <v>100</v>
@@ -1692,10 +1782,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2">
         <v>250</v>
@@ -1716,7 +1806,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -1725,7 +1815,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I11" s="5">
         <v>1</v>
@@ -1738,10 +1828,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -1759,10 +1849,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -1804,7 +1894,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,7 +1914,7 @@
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -1875,16 +1965,16 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2">
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="5"/>
@@ -1897,19 +1987,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="5"/>
@@ -1922,10 +2012,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2">
         <v>255</v>
@@ -1946,7 +2036,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2">
         <v>100</v>
@@ -1964,10 +2054,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -1976,7 +2066,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I8" s="5">
         <v>2</v>
@@ -1989,10 +2079,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -2013,7 +2103,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -2022,7 +2112,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I10" s="5">
         <v>1</v>
@@ -2038,7 +2128,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -2047,7 +2137,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I11" s="5">
         <v>1</v>
@@ -2060,10 +2150,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -2081,10 +2171,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -2146,7 +2236,7 @@
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2194,22 +2284,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D4" s="2">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -2221,10 +2311,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
         <v>10</v>
@@ -2242,10 +2332,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2">
         <v>50</v>
@@ -2263,10 +2353,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2">
         <v>200</v>
@@ -2287,7 +2377,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -2296,7 +2386,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8" s="5">
         <v>1</v>
@@ -2425,7 +2515,7 @@
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2473,22 +2563,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -2500,10 +2590,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2">
         <v>50</v>
@@ -2521,10 +2611,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2">
         <v>50</v>
@@ -2545,7 +2635,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2">
         <v>50</v>
@@ -2566,7 +2656,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
         <v>50</v>
@@ -2587,7 +2677,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2">
         <v>150</v>
@@ -2605,10 +2695,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -2617,7 +2707,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I10" s="5">
         <v>2</v>
@@ -2633,7 +2723,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -2642,7 +2732,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I11" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Update: add some columns for user table
</commit_message>
<xml_diff>
--- a/DB/DB.xlsx
+++ b/DB/DB.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="71">
   <si>
     <t>DB NAME</t>
   </si>
@@ -233,6 +233,15 @@
   </si>
   <si>
     <t>0: not confirmed,1: activated, 2: deactivated</t>
+  </si>
+  <si>
+    <t>sign_contract</t>
+  </si>
+  <si>
+    <t>confirm_payment_code</t>
+  </si>
+  <si>
+    <t>0: unsign, 1: signed</t>
   </si>
 </sst>
 </file>
@@ -580,7 +589,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:J21" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:J23" totalsRowShown="0" headerRowDxfId="54">
   <tableColumns count="10">
     <tableColumn id="1" name="Stt" dataDxfId="53">
       <calculatedColumnFormula>ROW()-3</calculatedColumnFormula>
@@ -1188,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:I15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,7 +1526,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1529,10 +1538,10 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="6"/>
     </row>
@@ -1542,19 +1551,23 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1</v>
+      </c>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1563,23 +1576,19 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18" s="5">
-        <v>1</v>
-      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1588,23 +1597,19 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0</v>
-      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1613,19 +1618,23 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1</v>
+      </c>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1634,20 +1643,66 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
       <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <f t="shared" ref="A22:A23" si="1">ROW()-3</f>
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Update: add payment email column
</commit_message>
<xml_diff>
--- a/DB/DB.xlsx
+++ b/DB/DB.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="73">
   <si>
     <t>DB NAME</t>
   </si>
@@ -151,9 +151,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>1: Main(Login), 2: child</t>
-  </si>
-  <si>
     <t>configuration</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>prefix</t>
   </si>
   <si>
-    <t>agree</t>
-  </si>
-  <si>
     <t>refer</t>
   </si>
   <si>
@@ -242,6 +236,18 @@
   </si>
   <si>
     <t>0: unsign, 1: signed</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>for future</t>
+  </si>
+  <si>
+    <t>payment_email</t>
   </si>
 </sst>
 </file>
@@ -589,7 +595,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:J23" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:J25" totalsRowShown="0" headerRowDxfId="54">
   <tableColumns count="10">
     <tableColumn id="1" name="Stt" dataDxfId="53">
       <calculatedColumnFormula>ROW()-3</calculatedColumnFormula>
@@ -629,7 +635,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A3:J14" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A3:J13" totalsRowShown="0" headerRowDxfId="32">
   <tableColumns count="10">
     <tableColumn id="1" name="Stt" dataDxfId="31">
       <calculatedColumnFormula>ROW()-3</calculatedColumnFormula>
@@ -1020,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -1029,7 +1035,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -1197,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1270,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A20" si="0">ROW()-3</f>
+        <f t="shared" ref="A4:A22" si="0">ROW()-3</f>
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1295,7 +1301,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -1316,7 +1322,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -1337,7 +1343,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -1358,7 +1364,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -1442,7 +1448,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>23</v>
@@ -1479,18 +1485,18 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <f t="shared" si="0"/>
+      <c r="A14" s="11">
+        <f>ROW()-3</f>
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1505,13 +1511,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="2">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1526,23 +1532,17 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0</v>
-      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1551,23 +1551,19 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="5">
-        <v>1</v>
-      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1576,19 +1572,23 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1597,19 +1597,23 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="H19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1</v>
+      </c>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1618,91 +1622,133 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="5">
-        <v>1</v>
-      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
-        <f>ROW()-3</f>
+      <c r="A21" s="4">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" s="5">
-        <v>0</v>
-      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
-        <f t="shared" ref="A22:A23" si="1">ROW()-3</f>
+      <c r="A22" s="4">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1</v>
+      </c>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
-        <f t="shared" si="1"/>
+        <f>ROW()-3</f>
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
       <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <f t="shared" ref="A24:A25" si="1">ROW()-3</f>
+        <v>21</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1880,7 +1926,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -1968,7 +2014,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>25</v>
@@ -1989,7 +2035,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>25</v>
@@ -2031,10 +2077,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2144,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A13" si="0">ROW()-3</f>
+        <f t="shared" ref="A4:A12" si="0">ROW()-3</f>
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2206,10 +2252,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="5" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="I8" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="6"/>
     </row>
@@ -2219,7 +2265,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
@@ -2230,8 +2276,12 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2240,7 +2290,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -2252,7 +2302,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I10" s="5">
         <v>1</v>
@@ -2265,23 +2315,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1</v>
-      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2306,37 +2352,16 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2376,7 +2401,7 @@
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2424,10 +2449,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2">
         <v>10</v>
@@ -2451,7 +2476,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -2472,7 +2497,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -2493,7 +2518,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -2655,7 +2680,7 @@
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2703,10 +2728,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2">
         <v>10</v>
@@ -2730,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -2751,7 +2776,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -2835,7 +2860,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -2847,7 +2872,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
Update: fix some columns of channel
</commit_message>
<xml_diff>
--- a/DB/DB.xlsx
+++ b/DB/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table List" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="75">
   <si>
     <t>DB NAME</t>
   </si>
@@ -145,9 +145,6 @@
     <t>channel_id</t>
   </si>
   <si>
-    <t>channel_name</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>update_at</t>
   </si>
   <si>
-    <t>updat_at</t>
-  </si>
-  <si>
     <t>pin_code</t>
   </si>
   <si>
@@ -248,6 +242,18 @@
   </si>
   <si>
     <t>payment_email</t>
+  </si>
+  <si>
+    <t>1: Approved, 2: Suspended, 3: Pending, 4: Blocked</t>
+  </si>
+  <si>
+    <t>daily_channel_id</t>
+  </si>
+  <si>
+    <t>daily_channel_name</t>
+  </si>
+  <si>
+    <t>daily_channel_username</t>
   </si>
 </sst>
 </file>
@@ -635,7 +641,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A3:J13" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="A3:J15" totalsRowShown="0" headerRowDxfId="32">
   <tableColumns count="10">
     <tableColumn id="1" name="Stt" dataDxfId="31">
       <calculatedColumnFormula>ROW()-3</calculatedColumnFormula>
@@ -1026,7 +1032,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -1035,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
@@ -1205,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1301,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -1322,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -1343,7 +1349,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -1364,7 +1370,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -1448,7 +1454,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>23</v>
@@ -1490,7 +1496,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>23</v>
@@ -1532,10 +1538,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1551,7 +1557,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>23</v>
@@ -1572,7 +1578,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
@@ -1584,7 +1590,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I18" s="5">
         <v>0</v>
@@ -1597,7 +1603,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
@@ -1609,7 +1615,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I19" s="5">
         <v>1</v>
@@ -1622,7 +1628,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>23</v>
@@ -1643,7 +1649,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
@@ -1701,7 +1707,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I23" s="5">
         <v>0</v>
@@ -1714,7 +1720,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>25</v>
@@ -1735,7 +1741,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>25</v>
@@ -1926,7 +1932,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -2014,7 +2020,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>25</v>
@@ -2035,7 +2041,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>25</v>
@@ -2077,16 +2083,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
@@ -2143,12 +2149,12 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <f t="shared" ref="A4:A12" si="0">ROW()-3</f>
+      <c r="A4" s="11">
+        <f>ROW()-3</f>
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
@@ -2162,31 +2168,29 @@
       <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A5:A14" si="0">ROW()-3</f>
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2">
-        <v>100</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -2198,13 +2202,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="2">
-        <v>255</v>
+        <v>100</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -2214,12 +2218,12 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <f t="shared" si="0"/>
+      <c r="A7" s="11">
+        <f>ROW()-3</f>
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -2240,23 +2244,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1</v>
-      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2265,23 +2265,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="5">
-        <v>1</v>
-      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2290,7 +2286,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -2302,7 +2298,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="I10" s="5">
         <v>1</v>
@@ -2315,19 +2311,23 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="5">
+        <v>3</v>
+      </c>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2336,32 +2336,78 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -2401,7 +2447,7 @@
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2449,10 +2495,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2">
         <v>10</v>
@@ -2476,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -2497,7 +2543,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -2518,7 +2564,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -2680,7 +2726,7 @@
     <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2728,10 +2774,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2">
         <v>10</v>
@@ -2755,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -2776,7 +2822,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -2860,7 +2906,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -2872,7 +2918,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
- Update: add some columns for net_admin table
</commit_message>
<xml_diff>
--- a/DB/DB.xlsx
+++ b/DB/DB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Table List" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="76">
   <si>
     <t>DB NAME</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>daily_channel_username</t>
+  </si>
+  <si>
+    <t>'/assets/img/logo.png'</t>
   </si>
 </sst>
 </file>
@@ -2085,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2770,7 +2773,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f t="shared" ref="A4:A11" si="0">ROW()-3</f>
+        <f t="shared" ref="A4:A14" si="0">ROW()-3</f>
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2843,18 +2846,20 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="I7" s="5"/>
       <c r="J7" s="6"/>
     </row>
@@ -2864,7 +2869,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -2885,13 +2890,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="2">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -2906,23 +2911,19 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="5">
-        <v>2</v>
-      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2931,7 +2932,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
@@ -2943,30 +2944,52 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="5" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="I11" s="5">
+        <v>2</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -2975,10 +2998,19 @@
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>

</xml_diff>